<commit_message>
added new data to PRVDRS
</commit_message>
<xml_diff>
--- a/data/Sistema_de_Notificacion_de_Muertes_Violentas/snmvTasas.xlsx
+++ b/data/Sistema_de_Notificacion_de_Muertes_Violentas/snmvTasas.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29725"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dashboard Version 27 de junio\Dashboard\Website\PARE_IND\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Sistema_de_Notificacion_de_Muertes_Violentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_71AF83F91C1526A707C65E167A846BCA8F270C91" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="1476" yWindow="1848" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AS" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -62,7 +74,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
@@ -391,22 +403,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="1" max="1" width="10.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>2017</v>
       </c>
@@ -434,7 +446,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2018</v>
       </c>
@@ -448,7 +460,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>2019</v>
       </c>
@@ -462,7 +474,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -476,7 +488,7 @@
         <v>3325284</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2018</v>
       </c>
@@ -490,7 +502,7 @@
         <v>3193344</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2019</v>
       </c>
@@ -504,7 +516,7 @@
         <v>3193553</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2017</v>
       </c>
@@ -518,7 +530,7 @@
         <v>21.592140701365658</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2018</v>
       </c>
@@ -532,7 +544,7 @@
         <v>20.667989417989418</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2019</v>
       </c>
@@ -546,7 +558,7 @@
         <v>19.664618060198155</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>2017</v>
       </c>
@@ -560,7 +572,7 @@
         <v>22.820325852552742</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>2018</v>
       </c>
@@ -574,7 +586,7 @@
         <v>22.460686161612784</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>2019</v>
       </c>
@@ -588,7 +600,7 @@
         <v>21.31249809642858</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>2017</v>
       </c>
@@ -602,7 +614,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>2018</v>
       </c>
@@ -616,7 +628,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>2019</v>
       </c>
@@ -630,7 +642,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>2017</v>
       </c>
@@ -644,7 +656,7 @@
         <v>1580779</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2018</v>
       </c>
@@ -658,7 +670,7 @@
         <v>1517003</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2019</v>
       </c>
@@ -672,7 +684,7 @@
         <v>1515598</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>2017</v>
       </c>
@@ -686,7 +698,7 @@
         <v>43.206545633513606</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>2018</v>
       </c>
@@ -700,7 +712,7 @@
         <v>40.013104786213347</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>2019</v>
       </c>
@@ -714,7 +726,7 @@
         <v>38.73058687066095</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>2017</v>
       </c>
@@ -728,7 +740,7 @@
         <v>44.853474697765961</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>2018</v>
       </c>
@@ -742,7 +754,7 @@
         <v>42.41510393484154</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>2019</v>
       </c>
@@ -756,7 +768,7 @@
         <v>40.861349216187925</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>2017</v>
       </c>
@@ -770,7 +782,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>2018</v>
       </c>
@@ -784,7 +796,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>2019</v>
       </c>
@@ -798,7 +810,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>2017</v>
       </c>
@@ -812,7 +824,7 @@
         <v>1744505</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>2018</v>
       </c>
@@ -826,7 +838,7 @@
         <v>1676341</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>2019</v>
       </c>
@@ -840,7 +852,7 @@
         <v>1677955</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>2017</v>
       </c>
@@ -854,7 +866,7 @@
         <v>2.0062997813133236</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>2018</v>
       </c>
@@ -868,7 +880,7 @@
         <v>3.1616478986077414</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>2019</v>
       </c>
@@ -882,7 +894,7 @@
         <v>2.4434505096978167</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>2017</v>
       </c>
@@ -896,7 +908,7 @@
         <v>1.9510101040238941</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>2018</v>
       </c>
@@ -910,7 +922,7 @@
         <v>3.5600915346314519</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>2019</v>
       </c>

</xml_diff>